<commit_message>
refactor and extend tests for Excel file reading
</commit_message>
<xml_diff>
--- a/src/test/resources/testobjectmodeldefinition.xlsx
+++ b/src/test/resources/testobjectmodeldefinition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/stuff/objectmodeldiagramgenerator/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3F6607-F01A-3540-B885-24BB83E66DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB8C0C2-7131-B14A-9CF8-1C64AF52AC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" activeTab="3" xr2:uid="{EA4244F2-FE33-7643-A566-43DD5B4E5092}"/>
   </bookViews>
@@ -16,9 +16,10 @@
     <sheet name="transitionstates" sheetId="19" r:id="rId1"/>
     <sheet name="scenarios" sheetId="22" r:id="rId2"/>
     <sheet name="businessevents" sheetId="1" r:id="rId3"/>
-    <sheet name="oms_OkSequence1_state1" sheetId="2" r:id="rId4"/>
-    <sheet name="doc_entities-and-attribute" sheetId="3" r:id="rId5"/>
-    <sheet name="doc_conventions" sheetId="4" r:id="rId6"/>
+    <sheet name="oms_OkSequence_state1" sheetId="2" r:id="rId4"/>
+    <sheet name="oms_OkSequence_state2" sheetId="23" r:id="rId5"/>
+    <sheet name="doc_entities-and-attribute" sheetId="3" r:id="rId6"/>
+    <sheet name="doc_conventions" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="185">
   <si>
     <t>PartOfTheWorld</t>
   </si>
@@ -757,7 +758,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -799,6 +800,12 @@
     <xf numFmtId="49" fontId="3" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -833,7 +840,32 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -1069,24 +1101,24 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{422A6A28-4F84-CA4D-BC76-24F29CBA51D2}" name="Tabelle1" displayName="Tabelle1" ref="A1:C10" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{422A6A28-4F84-CA4D-BC76-24F29CBA51D2}" name="Tabelle1" displayName="Tabelle1" ref="A1:C10" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:C10" xr:uid="{422A6A28-4F84-CA4D-BC76-24F29CBA51D2}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E843E1F4-E64E-684F-A053-BC1EBA87FC3D}" name="Key" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{AD27EB56-E6EA-1B48-8FF5-F0DBDD95396F}" name="Description" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{3568C30F-FCC2-614D-B4C9-3748BE4A945B}" name="ScenarioKey" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{E843E1F4-E64E-684F-A053-BC1EBA87FC3D}" name="Key" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{AD27EB56-E6EA-1B48-8FF5-F0DBDD95396F}" name="Description" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{3568C30F-FCC2-614D-B4C9-3748BE4A945B}" name="ScenarioKey" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C4839BD3-5D73-734A-B902-529B029081C5}" name="Tabelle2" displayName="Tabelle2" ref="A1:C17" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C4839BD3-5D73-734A-B902-529B029081C5}" name="Tabelle2" displayName="Tabelle2" ref="A1:C17" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:C17" xr:uid="{C4839BD3-5D73-734A-B902-529B029081C5}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{CD4C934D-C638-6641-9429-0635496C9CA8}" name="Convention" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{49EAB0E3-F001-BB4E-9093-217E47E4FDA4}" name="Description" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{2C6C41A4-B550-2949-BD2B-0FF7B652198B}" name="Reasoning" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{CD4C934D-C638-6641-9429-0635496C9CA8}" name="Convention" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{49EAB0E3-F001-BB4E-9093-217E47E4FDA4}" name="Description" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{2C6C41A4-B550-2949-BD2B-0FF7B652198B}" name="Reasoning" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1549,7 +1581,7 @@
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1685,7 +1717,7 @@
   <dimension ref="A1:AB16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
@@ -1703,90 +1735,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="22" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22"/>
-      <c r="X1" s="22"/>
-      <c r="Y1" s="15" t="s">
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
+      <c r="AB1" s="17"/>
     </row>
     <row r="2" spans="1:28" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="20" t="s">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20" t="s">
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20" t="s">
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="21" t="s">
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21" t="s">
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="21"/>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="16" t="s">
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="Z2" s="16"/>
-      <c r="AA2" s="16"/>
-      <c r="AB2" s="16"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
     </row>
     <row r="3" spans="1:28" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="24"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="26"/>
       <c r="C3" s="11" t="s">
         <v>149</v>
       </c>
@@ -3000,22 +3032,22 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A4:I4 I5:I6 J4:AB6 I7:AB7 I8:XFD9 A5:H9 A10:XFD1048576">
-    <cfRule type="containsBlanks" dxfId="3" priority="5" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="5" priority="5" stopIfTrue="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:I4 C5:H9 I5:I6 J4:AB6 I7:AB7 I8:XFD9 C10:XFD1048576">
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="notEqual">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC1:XFD7">
-    <cfRule type="containsBlanks" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="3" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(AC1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC1:XFD7">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3036,6 +3068,318 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25808B99-ED80-D243-97F2-A9C93ED14454}">
+  <dimension ref="A1:AB4"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="1" customWidth="1"/>
+    <col min="3" max="17" width="10.83203125" style="1" customWidth="1"/>
+    <col min="18" max="24" width="8.6640625" style="1" customWidth="1"/>
+    <col min="25" max="26" width="10.83203125" style="1"/>
+    <col min="27" max="27" width="15.5" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
+      <c r="AB1" s="17"/>
+    </row>
+    <row r="2" spans="1:28" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
+    </row>
+    <row r="3" spans="1:28" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="21"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="O3" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="P3" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q3" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="R3" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="S3" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="T3" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="U3" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="V3" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="W3" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="X3" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="Y3" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="Z3" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA3" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB3" s="14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="Y2:AB2"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="N1:X1"/>
+    <mergeCell ref="Y1:AB1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R2:X2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A4:AB4 AC1:XFD4 A5:XFD1048576">
+    <cfRule type="containsBlanks" dxfId="1" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:AB4 AC1:XFD4 C5:XFD1048576">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="notEqual">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{543A8520-1C60-0F49-AC37-D480DFC011B5}">
+          <x14:formula1>
+            <xm:f>businessevents!$A$2:$A$65</xm:f>
+          </x14:formula1>
+          <xm:sqref>A4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF36908E-7B0D-AC4C-AAB6-F6FFCB9AE073}">
   <dimension ref="A1:D25"/>
   <sheetViews>
@@ -3406,7 +3750,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{957B1B1D-C2EE-9B4D-B3FF-AD115CBB19B4}">
   <dimension ref="A1:C17"/>
   <sheetViews>

</xml_diff>

<commit_message>
update scen seq service
</commit_message>
<xml_diff>
--- a/src/test/resources/testobjectmodeldefinition.xlsx
+++ b/src/test/resources/testobjectmodeldefinition.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/stuff/objectmodeldiagramgenerator/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852AB063-BC64-B34E-B46C-6C2F13434204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AA8566-4E19-C941-9786-3D86D7F24CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" activeTab="5" xr2:uid="{EA4244F2-FE33-7643-A566-43DD5B4E5092}"/>
   </bookViews>
@@ -653,9 +653,6 @@
     <t>event0502</t>
   </si>
   <si>
-    <t>scenario1, scenario4</t>
-  </si>
-  <si>
     <t>The first house is built, and then Anton moves in to the first floor.</t>
   </si>
   <si>
@@ -843,6 +840,9 @@
   </si>
   <si>
     <t>Charlie C</t>
+  </si>
+  <si>
+    <t>scenario1, scenario3, scenario4</t>
   </si>
 </sst>
 </file>
@@ -1099,10 +1099,16 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1114,35 +1120,48 @@
     <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="29">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -1435,25 +1454,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1643,24 +1643,24 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F5B660FE-5499-6D4F-B192-6D495D38DF3B}" name="Tabelle17" displayName="Tabelle17" ref="A1:C13" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F5B660FE-5499-6D4F-B192-6D495D38DF3B}" name="Tabelle17" displayName="Tabelle17" ref="A1:C13" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A1:C13" xr:uid="{422A6A28-4F84-CA4D-BC76-24F29CBA51D2}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{938701D0-9835-4745-A220-8C6068F221FF}" name="Key" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{381D88C7-4F57-284F-9F9B-E9AEB9E0E9F8}" name="Description" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{0A673B68-A98A-1B41-889D-06C26B97C1F1}" name="ScenarioKey" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{938701D0-9835-4745-A220-8C6068F221FF}" name="Key" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{381D88C7-4F57-284F-9F9B-E9AEB9E0E9F8}" name="Description" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{0A673B68-A98A-1B41-889D-06C26B97C1F1}" name="ScenarioKey" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C4839BD3-5D73-734A-B902-529B029081C5}" name="Tabelle2" displayName="Tabelle2" ref="A1:C17" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C4839BD3-5D73-734A-B902-529B029081C5}" name="Tabelle2" displayName="Tabelle2" ref="A1:C17" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:C17" xr:uid="{C4839BD3-5D73-734A-B902-529B029081C5}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{CD4C934D-C638-6641-9429-0635496C9CA8}" name="Convention" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{49EAB0E3-F001-BB4E-9093-217E47E4FDA4}" name="Description" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{2C6C41A4-B550-2949-BD2B-0FF7B652198B}" name="Reasoning" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{CD4C934D-C638-6641-9429-0635496C9CA8}" name="Convention" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{49EAB0E3-F001-BB4E-9093-217E47E4FDA4}" name="Description" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{2C6C41A4-B550-2949-BD2B-0FF7B652198B}" name="Reasoning" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1994,7 +1994,7 @@
         <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2005,7 +2005,7 @@
         <v>106</v>
       </c>
       <c r="C3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2016,7 +2016,7 @@
         <v>106</v>
       </c>
       <c r="C4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -2820,7 +2820,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2849,7 +2849,7 @@
         <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2860,7 +2860,7 @@
         <v>112</v>
       </c>
       <c r="C3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2882,7 +2882,7 @@
         <v>112</v>
       </c>
       <c r="C5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2890,10 +2890,10 @@
         <v>116</v>
       </c>
       <c r="B6" t="s">
-        <v>203</v>
+        <v>266</v>
       </c>
       <c r="C6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -2983,7 +2983,7 @@
         <v>187</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>113</v>
@@ -3015,7 +3015,7 @@
       <c r="A9" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="19" t="s">
         <v>201</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -3037,7 +3037,7 @@
       <c r="A11" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="19" t="s">
         <v>198</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -3045,22 +3045,22 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="B12" s="31" t="s">
-        <v>220</v>
+      <c r="B12" s="21" t="s">
+        <v>219</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="B13" s="29" t="s">
-        <v>256</v>
+      <c r="B13" s="19" t="s">
+        <v>255</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>116</v>
@@ -3084,7 +3084,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="A12" sqref="A12:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3106,113 +3106,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="24" t="s">
         <v>108</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D1" s="27"/>
       <c r="E1" s="27"/>
       <c r="F1" s="27"/>
       <c r="G1" s="27"/>
       <c r="H1" s="27"/>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+    </row>
+    <row r="2" spans="1:18" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+    </row>
+    <row r="3" spans="1:18" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="17" t="s">
         <v>208</v>
-      </c>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-    </row>
-    <row r="2" spans="1:18" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="24" t="s">
-        <v>226</v>
-      </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24" t="s">
-        <v>227</v>
-      </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="25" t="s">
-        <v>228</v>
-      </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25" t="s">
-        <v>231</v>
-      </c>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25" t="s">
-        <v>259</v>
-      </c>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-    </row>
-    <row r="3" spans="1:18" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="17" t="s">
-        <v>209</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>8</v>
       </c>
       <c r="K3" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="M3" s="18" t="s">
         <v>222</v>
       </c>
-      <c r="L3" s="18" t="s">
+      <c r="N3" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="O3" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="P3" s="18" t="s">
         <v>257</v>
       </c>
-      <c r="M3" s="18" t="s">
+      <c r="Q3" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="R3" s="18" t="s">
         <v>223</v>
-      </c>
-      <c r="N3" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="O3" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="P3" s="18" t="s">
-        <v>258</v>
-      </c>
-      <c r="Q3" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="R3" s="18" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:18" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3223,13 +3223,13 @@
         <v>110</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>37</v>
@@ -3288,13 +3288,13 @@
         <v>37</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>37</v>
@@ -3344,13 +3344,13 @@
         <v>37</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>37</v>
@@ -3409,13 +3409,13 @@
         <v>37</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>37</v>
@@ -3474,16 +3474,16 @@
         <v>37</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P8" s="3" t="s">
         <v>37</v>
@@ -3521,13 +3521,13 @@
         <v>37</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>37</v>
@@ -3598,13 +3598,13 @@
         <v>37</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="17" x14ac:dyDescent="0.2">
@@ -3642,16 +3642,16 @@
         <v>37</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P11" s="3" t="s">
         <v>37</v>
@@ -3671,13 +3671,13 @@
         <v>110</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>239</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>240</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>37</v>
@@ -3736,13 +3736,13 @@
         <v>37</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>37</v>
@@ -3792,13 +3792,13 @@
         <v>37</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>37</v>
@@ -3848,13 +3848,13 @@
         <v>37</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>37</v>
@@ -3904,13 +3904,13 @@
         <v>37</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>37</v>
@@ -3978,16 +3978,16 @@
         <v>37</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P17" s="3" t="s">
         <v>37</v>
@@ -4034,16 +4034,16 @@
         <v>37</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P18" s="3" t="s">
         <v>37</v>
@@ -4090,7 +4090,7 @@
         <v>37</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M19" s="3" t="s">
         <v>37</v>
@@ -4146,7 +4146,7 @@
         <v>37</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M20" s="3" t="s">
         <v>37</v>
@@ -4193,13 +4193,13 @@
         <v>37</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>37</v>
@@ -4258,16 +4258,16 @@
         <v>37</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P22" s="3" t="s">
         <v>37</v>
@@ -4314,16 +4314,16 @@
         <v>37</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="P23" s="3" t="s">
         <v>37</v>
@@ -4370,7 +4370,7 @@
         <v>37</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="M24" s="3" t="s">
         <v>37</v>
@@ -4408,7 +4408,7 @@
         <v>37</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>37</v>
@@ -4464,7 +4464,7 @@
         <v>37</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>37</v>
@@ -4511,7 +4511,7 @@
         <v>164</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>37</v>
@@ -4573,22 +4573,22 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="S8:XFD21 P22:XFD24 A4:R24 A25:XFD1048576">
-    <cfRule type="containsBlanks" dxfId="13" priority="3" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="18" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S8:XFD21 P22:XFD24 C4:R24 C25:XFD1048576">
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:XFD7">
-    <cfRule type="containsBlanks" dxfId="11" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="16" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(S1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:XFD7">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4629,113 +4629,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="24" t="s">
         <v>108</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D1" s="27"/>
       <c r="E1" s="27"/>
       <c r="F1" s="27"/>
       <c r="G1" s="27"/>
       <c r="H1" s="27"/>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+    </row>
+    <row r="2" spans="1:18" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+    </row>
+    <row r="3" spans="1:18" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="17" t="s">
         <v>208</v>
-      </c>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-    </row>
-    <row r="2" spans="1:18" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="24" t="s">
-        <v>226</v>
-      </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24" t="s">
-        <v>227</v>
-      </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="25" t="s">
-        <v>228</v>
-      </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25" t="s">
-        <v>231</v>
-      </c>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25" t="s">
-        <v>259</v>
-      </c>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-    </row>
-    <row r="3" spans="1:18" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="17" t="s">
-        <v>209</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>8</v>
       </c>
       <c r="K3" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="M3" s="18" t="s">
         <v>222</v>
       </c>
-      <c r="L3" s="18" t="s">
+      <c r="N3" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="O3" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="P3" s="18" t="s">
         <v>257</v>
       </c>
-      <c r="M3" s="18" t="s">
+      <c r="Q3" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="R3" s="18" t="s">
         <v>223</v>
-      </c>
-      <c r="N3" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="O3" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="P3" s="18" t="s">
-        <v>258</v>
-      </c>
-      <c r="Q3" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="R3" s="18" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:18" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -4746,13 +4746,13 @@
         <v>110</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>37</v>
@@ -4807,22 +4807,22 @@
     <mergeCell ref="P2:R2"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:R4 A5:XFD1048576">
-    <cfRule type="containsBlanks" dxfId="9" priority="3" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="14" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:R4 C5:XFD1048576">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:XFD4">
-    <cfRule type="containsBlanks" dxfId="7" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="12" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(S1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:XFD4">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4853,10 +4853,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="24" t="s">
         <v>108</v>
       </c>
       <c r="C1" s="27" t="s">
@@ -4872,71 +4872,71 @@
       <c r="K1" s="27"/>
       <c r="L1" s="27"/>
       <c r="M1" s="27"/>
-      <c r="N1" s="26" t="s">
+      <c r="N1" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="19" t="s">
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="19"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
     </row>
     <row r="2" spans="1:28" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="24" t="s">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24" t="s">
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="25" t="s">
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25" t="s">
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
-      <c r="V2" s="25"/>
-      <c r="W2" s="25"/>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="20" t="s">
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="Z2" s="20"/>
-      <c r="AA2" s="20"/>
-      <c r="AB2" s="20"/>
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="31"/>
+      <c r="AB2" s="31"/>
     </row>
     <row r="3" spans="1:28" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="28"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
       <c r="C3" s="11" t="s">
         <v>129</v>
       </c>
@@ -6150,22 +6150,22 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A4:I4 I5:I6 J4:AB6 I7:AB7 I8:XFD9 A5:H9 A10:XFD1048576">
-    <cfRule type="containsBlanks" dxfId="5" priority="5" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="10" priority="5" stopIfTrue="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:I4 C5:H9 I5:I6 J4:AB6 I7:AB7 I8:XFD9 C10:XFD1048576">
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="notEqual">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC1:XFD7">
-    <cfRule type="containsBlanks" dxfId="3" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="8" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(AC1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC1:XFD7">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6208,10 +6208,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="24" t="s">
         <v>108</v>
       </c>
       <c r="C1" s="27" t="s">
@@ -6227,71 +6227,71 @@
       <c r="K1" s="27"/>
       <c r="L1" s="27"/>
       <c r="M1" s="27"/>
-      <c r="N1" s="26" t="s">
+      <c r="N1" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="19" t="s">
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="19"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
     </row>
     <row r="2" spans="1:28" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="24" t="s">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24" t="s">
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="25" t="s">
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25" t="s">
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
-      <c r="V2" s="25"/>
-      <c r="W2" s="25"/>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="20" t="s">
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="Z2" s="20"/>
-      <c r="AA2" s="20"/>
-      <c r="AB2" s="20"/>
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="31"/>
+      <c r="AB2" s="31"/>
     </row>
     <row r="3" spans="1:28" s="3" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="28"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
       <c r="C3" s="15" t="s">
         <v>129</v>
       </c>
@@ -6472,12 +6472,12 @@
     <mergeCell ref="R2:X2"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:AB4 AC1:XFD4 A5:XFD1048576">
-    <cfRule type="containsBlanks" dxfId="1" priority="3" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="6" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:AB4 AC1:XFD4 C5:XFD1048576">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6656,18 +6656,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6689,6 +6689,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44EA3924-C60D-4AB3-8333-F249729C0DDD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2124C44-2049-4194-ADAF-B2DF55B36692}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -6702,12 +6710,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44EA3924-C60D-4AB3-8333-F249729C0DDD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix handling empty rows
</commit_message>
<xml_diff>
--- a/src/test/resources/testobjectmodeldefinition.xlsx
+++ b/src/test/resources/testobjectmodeldefinition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/stuff/objectmodeldiagramgenerator/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC2EFDF-9574-4A4E-837A-E17707F50489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DD609D-529F-0649-8BAF-A291B432290E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{EA4244F2-FE33-7643-A566-43DD5B4E5092}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" activeTab="1" xr2:uid="{EA4244F2-FE33-7643-A566-43DD5B4E5092}"/>
   </bookViews>
   <sheets>
     <sheet name="transitionstates" sheetId="19" r:id="rId1"/>
@@ -860,8 +860,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{22601192-491E-8F4D-9C10-C176E33BD4E0}" name="Table4" displayName="Table4" ref="A1:C4" totalsRowShown="0">
-  <autoFilter ref="A1:C4" xr:uid="{22601192-491E-8F4D-9C10-C176E33BD4E0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{22601192-491E-8F4D-9C10-C176E33BD4E0}" name="Table4" displayName="Table4" ref="A1:C6" totalsRowShown="0">
+  <autoFilter ref="A1:C6" xr:uid="{22601192-491E-8F4D-9C10-C176E33BD4E0}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E784BCB2-FBAB-744E-A8F7-FC6F72D93FEA}" name="Key"/>
     <tableColumn id="2" xr3:uid="{874EA81C-43B9-1B40-B7EB-E7A32412DA03}" name="PredecessorKey"/>
@@ -872,8 +872,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C65736A8-A876-BF4F-814D-17C23A5FCFB6}" name="Table364" displayName="Table364" ref="A1:C15" totalsRowShown="0">
-  <autoFilter ref="A1:C15" xr:uid="{C0682A79-088A-6444-B944-088363065AF9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C65736A8-A876-BF4F-814D-17C23A5FCFB6}" name="Table364" displayName="Table364" ref="A1:C19" totalsRowShown="0">
+  <autoFilter ref="A1:C19" xr:uid="{C0682A79-088A-6444-B944-088363065AF9}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E5FCEA39-DE51-3646-820E-D0F1B70B5564}" name="Key"/>
     <tableColumn id="2" xr3:uid="{CF2E014B-E327-CA40-902E-3C4B42B40F50}" name="PredecessorKeys"/>
@@ -884,8 +884,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F5B660FE-5499-6D4F-B192-6D495D38DF3B}" name="Tabelle17" displayName="Tabelle17" ref="A1:C13" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:C13" xr:uid="{422A6A28-4F84-CA4D-BC76-24F29CBA51D2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F5B660FE-5499-6D4F-B192-6D495D38DF3B}" name="Tabelle17" displayName="Tabelle17" ref="A1:C17" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:C17" xr:uid="{422A6A28-4F84-CA4D-BC76-24F29CBA51D2}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{938701D0-9835-4745-A220-8C6068F221FF}" name="Key" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{381D88C7-4F57-284F-9F9B-E9AEB9E0E9F8}" name="Description" dataDxfId="9"/>
@@ -1192,10 +1192,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E4C7D1-8068-2740-AEF0-32B40D504764}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1226,25 +1226,25 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>91</v>
-      </c>
-    </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1258,10 +1258,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6F5FAD2-8154-0D49-A79A-D1DF14B91F10}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1293,47 +1293,47 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>42</v>
-      </c>
-    </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B10" t="s">
         <v>104</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C10" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1349,11 +1349,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{223ACBB0-66D3-934A-A293-379036E0F203}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1408,23 +1408,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>14</v>
-      </c>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="8"/>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>14</v>
@@ -1432,10 +1426,10 @@
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>27</v>
+        <v>89</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>14</v>
@@ -1443,67 +1437,93 @@
     </row>
     <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B10" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C10" s="9" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="8"/>
+    </row>
+    <row r="13" spans="1:3" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B14" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C14" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B16" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C16" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B17" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C17" s="9" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add test data, update unit tests accordingly
</commit_message>
<xml_diff>
--- a/src/test/resources/testobjectmodeldefinition.xlsx
+++ b/src/test/resources/testobjectmodeldefinition.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/stuff/objectmodeldiagramgenerator/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DD609D-529F-0649-8BAF-A291B432290E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F2F8E5-08D3-A74C-B390-C04739FB5BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" activeTab="1" xr2:uid="{EA4244F2-FE33-7643-A566-43DD5B4E5092}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="businessevents" sheetId="25" r:id="rId3"/>
     <sheet name="oms_PersonsAndHouses_state1" sheetId="26" r:id="rId4"/>
     <sheet name="oms_PersonsAndHouses_state2" sheetId="27" r:id="rId5"/>
+    <sheet name="___oms_Persons_state1" sheetId="28" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="125">
   <si>
     <t>name</t>
   </si>
@@ -351,13 +352,73 @@
   </si>
   <si>
     <t>scenario1, scenario3, scenario4</t>
+  </si>
+  <si>
+    <t>scenario6</t>
+  </si>
+  <si>
+    <t>Anton, Berta, and Charlie become friends and get older.</t>
+  </si>
+  <si>
+    <t>event0601</t>
+  </si>
+  <si>
+    <t>Berta and Charlie become friends.</t>
+  </si>
+  <si>
+    <t>event0602</t>
+  </si>
+  <si>
+    <t>event0603</t>
+  </si>
+  <si>
+    <t>event0604</t>
+  </si>
+  <si>
+    <t>Anton joins Berta and Charlie's friendship.</t>
+  </si>
+  <si>
+    <t>Anton and Charlie get one year older.</t>
+  </si>
+  <si>
+    <t>update</t>
+  </si>
+  <si>
+    <t>p2p02</t>
+  </si>
+  <si>
+    <t>friendship</t>
+  </si>
+  <si>
+    <t>(berta, charlie)</t>
+  </si>
+  <si>
+    <t>scenario1, scenario2, scenario4</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>(anton, berta, charlie)</t>
+  </si>
+  <si>
+    <t>event0605</t>
+  </si>
+  <si>
+    <t>Anton and Berta get divorced.</t>
+  </si>
+  <si>
+    <t>After Anton, Berta, and Charlie celebrated a party, Anton and Charlie are not friends anymore.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -391,8 +452,14 @@
       <name val="Consolas"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -415,6 +482,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -547,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -592,6 +665,9 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -613,11 +689,67 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -884,12 +1016,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F5B660FE-5499-6D4F-B192-6D495D38DF3B}" name="Tabelle17" displayName="Tabelle17" ref="A1:C17" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:C17" xr:uid="{422A6A28-4F84-CA4D-BC76-24F29CBA51D2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F5B660FE-5499-6D4F-B192-6D495D38DF3B}" name="Tabelle17" displayName="Tabelle17" ref="A1:C23" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A1:C23" xr:uid="{422A6A28-4F84-CA4D-BC76-24F29CBA51D2}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{938701D0-9835-4745-A220-8C6068F221FF}" name="Key" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{381D88C7-4F57-284F-9F9B-E9AEB9E0E9F8}" name="Description" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{0A673B68-A98A-1B41-889D-06C26B97C1F1}" name="ScenarioKey" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{938701D0-9835-4745-A220-8C6068F221FF}" name="Key" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{381D88C7-4F57-284F-9F9B-E9AEB9E0E9F8}" name="Description" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{0A673B68-A98A-1B41-889D-06C26B97C1F1}" name="ScenarioKey" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1258,10 +1390,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6F5FAD2-8154-0D49-A79A-D1DF14B91F10}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1337,6 +1469,17 @@
         <v>56</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" t="s">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1349,17 +1492,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{223ACBB0-66D3-934A-A293-379036E0F203}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" style="3" customWidth="1"/>
-    <col min="2" max="2" width="93.1640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="96.6640625" style="7" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" style="7" customWidth="1"/>
     <col min="4" max="16384" width="11" style="5"/>
   </cols>
@@ -1525,6 +1668,66 @@
       </c>
       <c r="C17" s="9" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="8"/>
+    </row>
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1542,10 +1745,10 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12:A16"/>
+      <selection pane="bottomRight" activeCell="P10" sqref="P10:R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1567,66 +1770,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="21" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="22" t="s">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22" t="s">
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="15" t="s">
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15" t="s">
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15" t="s">
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
     </row>
     <row r="3" spans="1:18" s="2" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="10" t="s">
         <v>46</v>
       </c>
@@ -3034,22 +3237,22 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="S8:XFD21 P22:XFD24 A4:R24 A25:XFD1048576">
-    <cfRule type="containsBlanks" dxfId="7" priority="3" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="11" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S8:XFD21 P22:XFD24 C4:R24 C25:XFD1048576">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:XFD7">
-    <cfRule type="containsBlanks" dxfId="5" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="9" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(S1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:XFD7">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3090,66 +3293,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="21" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="22" t="s">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22" t="s">
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="15" t="s">
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15" t="s">
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15" t="s">
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
     </row>
     <row r="3" spans="1:18" s="2" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="10" t="s">
         <v>46</v>
       </c>
@@ -3268,22 +3471,22 @@
     <mergeCell ref="P2:R2"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:R4 A5:XFD1048576">
-    <cfRule type="containsBlanks" dxfId="3" priority="3" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="7" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:R4 C5:XFD1048576">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:XFD4">
-    <cfRule type="containsBlanks" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="5" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(S1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:XFD4">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3291,13 +3494,250 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B5D323E-2665-E041-95E7-E289DAEFE0FA}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="1" customWidth="1"/>
+    <col min="3" max="5" width="10.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="1:8" s="2" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="A4:E4 A5:XFD1048576">
+    <cfRule type="containsBlanks" dxfId="3" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:E4 C5:XFD1048576">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="notEqual">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:XFD4">
+    <cfRule type="containsBlanks" dxfId="1" priority="1" stopIfTrue="1">
+      <formula>LEN(TRIM(I1))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:XFD4">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="notEqual">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="E5:E6" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3459,15 +3899,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44EA3924-C60D-4AB3-8333-F249729C0DDD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2124C44-2049-4194-ADAF-B2DF55B36692}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="fe6e65e6-3f48-4872-a1e7-e48555659f5f"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3491,17 +3942,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2124C44-2049-4194-ADAF-B2DF55B36692}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44EA3924-C60D-4AB3-8333-F249729C0DDD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="fe6e65e6-3f48-4872-a1e7-e48555659f5f"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add test diagrams for scenario6, unit tests fail!
</commit_message>
<xml_diff>
--- a/src/test/resources/testobjectmodeldefinition.xlsx
+++ b/src/test/resources/testobjectmodeldefinition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/stuff/objectmodeldiagramgenerator/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F2F8E5-08D3-A74C-B390-C04739FB5BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D80C7D-93E4-284E-844C-F5944F20EA0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" activeTab="1" xr2:uid="{EA4244F2-FE33-7643-A566-43DD5B4E5092}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="businessevents" sheetId="25" r:id="rId3"/>
     <sheet name="oms_PersonsAndHouses_state1" sheetId="26" r:id="rId4"/>
     <sheet name="oms_PersonsAndHouses_state2" sheetId="27" r:id="rId5"/>
-    <sheet name="___oms_Persons_state1" sheetId="28" r:id="rId6"/>
+    <sheet name="oms_Persons_state1" sheetId="28" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="127">
   <si>
     <t>name</t>
   </si>
@@ -357,9 +357,6 @@
     <t>scenario6</t>
   </si>
   <si>
-    <t>Anton, Berta, and Charlie become friends and get older.</t>
-  </si>
-  <si>
     <t>event0601</t>
   </si>
   <si>
@@ -411,7 +408,16 @@
     <t>Anton and Berta get divorced.</t>
   </si>
   <si>
-    <t>After Anton, Berta, and Charlie celebrated a party, Anton and Charlie are not friends anymore.</t>
+    <t>predivorce</t>
+  </si>
+  <si>
+    <t>(anton, charlie)</t>
+  </si>
+  <si>
+    <t>After Anton, Berta, and Charlie celebrated a party, Berta leaves the friendship.</t>
+  </si>
+  <si>
+    <t>Anton, Berta, and Charlie become friends and get older. Then the situation changes again.</t>
   </si>
 </sst>
 </file>
@@ -665,6 +671,12 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -687,12 +699,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1393,7 +1399,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1474,10 +1480,10 @@
         <v>105</v>
       </c>
       <c r="B12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C12" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1495,8 +1501,8 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1677,56 +1683,56 @@
     </row>
     <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="B19" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="16" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C20" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" s="16" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="C21" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="16" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C22" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="C22" s="16" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="B23" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="16" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1745,7 +1751,7 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="P10" sqref="P10:R10"/>
@@ -1770,66 +1776,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="22" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="23" t="s">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23" t="s">
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="16" t="s">
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16" t="s">
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16" t="s">
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
     </row>
     <row r="3" spans="1:18" s="2" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="10" t="s">
         <v>46</v>
       </c>
@@ -3293,66 +3299,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="22" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="23" t="s">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23" t="s">
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="16" t="s">
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16" t="s">
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16" t="s">
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
     </row>
     <row r="3" spans="1:18" s="2" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="10" t="s">
         <v>46</v>
       </c>
@@ -3496,13 +3502,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B5D323E-2665-E041-95E7-E289DAEFE0FA}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3511,44 +3517,44 @@
     <col min="2" max="2" width="8" style="1" customWidth="1"/>
     <col min="3" max="5" width="10.83203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="20.5" style="1" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="16" t="s">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16" t="s">
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="15" t="s">
         <v>58</v>
       </c>
@@ -3570,7 +3576,7 @@
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>11</v>
@@ -3584,22 +3590,22 @@
       <c r="E4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="G4" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="H4" s="17" t="s">
         <v>116</v>
-      </c>
-      <c r="H4" s="25" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>97</v>
@@ -3608,7 +3614,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>1</v>
@@ -3622,10 +3628,10 @@
     </row>
     <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>99</v>
@@ -3634,7 +3640,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>1</v>
@@ -3648,54 +3654,106 @@
     </row>
     <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="G7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="G8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>117</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3735,9 +3793,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3899,26 +3960,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2124C44-2049-4194-ADAF-B2DF55B36692}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44EA3924-C60D-4AB3-8333-F249729C0DDD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="fe6e65e6-3f48-4872-a1e7-e48555659f5f"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3942,9 +3992,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44EA3924-C60D-4AB3-8333-F249729C0DDD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2124C44-2049-4194-ADAF-B2DF55B36692}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="fe6e65e6-3f48-4872-a1e7-e48555659f5f"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>